<commit_message>
Added the second unit tests for the InvestmentAccount Class and did some samll fixes with methods and the test plan.
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_investment_account.xlsx
+++ b/tests/A02_pixell_test_plan_investment_account.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4928f0ddc5ce2e2f/Documents/Red River College/2-Fall 2024/2. Intermediate Software Development/Project/isd_project/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{9D6AEFC8-F3D7-467B-9A12-00596A3BA98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{687F7095-B146-43DF-ABA5-66CCC9C2189E}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{9D6AEFC8-F3D7-467B-9A12-00596A3BA98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B4E6663-F111-46B4-9E41-568BC7C0F6B4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-12" yWindow="0" windowWidth="17904" windowHeight="12744" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -269,37 +269,37 @@
     <t>service_charge = 0.50</t>
   </si>
   <si>
+    <t>service_charge = 2.50</t>
+  </si>
+  <si>
+    <t>Account Number: 709 Balance: $450.00
+Date Created: 2016, 7, 9 Management fee: Waived
+Account Type: Investment</t>
+  </si>
+  <si>
+    <t>Account Number: 709 Balance: $450.00
+Date Created: 2016, 7, 9 Management fee: $2.00
+Account Type: Investment</t>
+  </si>
+  <si>
     <t>Account Number = 709
 Client Number = 9710
 Balance = 450
-Date Created = July 9, 2016
+Date Created = July 9, 2018
 management_fee = 2</t>
-  </si>
-  <si>
-    <t>service_charge = 2.50</t>
   </si>
   <si>
     <t>Account Number = 709
 Client Number = 9710
 Balance = 450
-Date Created = July 9, 2019
+Date Created = July 9, 2014
 management_fee = 2</t>
-  </si>
-  <si>
-    <t>Account Number: 709 Balance: $450.00
-Date Created: 2016, 7, 9 Management fee: Waived
-Account Type: Investment</t>
-  </si>
-  <si>
-    <t>Account Number: 709 Balance: $450.00
-Date Created: 2016, 7, 9 Management fee: $2.00
-Account Type: Investment</t>
   </si>
   <si>
     <t>Account Number = 709
 Client Number = 9710
 Balance = 450
-Date Created = July 9, 2022
+Date Created = July 9, 2011
 management_fee = 2</t>
   </si>
 </sst>
@@ -808,6 +808,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1207,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,7 +1293,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>23</v>
@@ -1329,7 +1333,7 @@
         <v>26</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>27</v>
@@ -1349,10 +1353,10 @@
         <v>26</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="84.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1369,10 +1373,10 @@
         <v>26</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="84.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1389,10 +1393,10 @@
         <v>26</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="84.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1409,10 +1413,10 @@
         <v>26</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>